<commit_message>
add  sceanrio creation  et  parametrage  de action
</commit_message>
<xml_diff>
--- a/resources/testData/TestData.xlsx
+++ b/resources/testData/TestData.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="815">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2453,6 +2453,81 @@
   </si>
   <si>
     <t>désignation action Quam eius est est cupiditate consequatur delectus pariatur. Fugit voluptatem quaerat quisquam autem sit. Quia quidem optio at in ut cumque.</t>
+  </si>
+  <si>
+    <t>désignation de modele action Quia inventore numquam qui veniam dolores rerum. Ipsam qui sit iusto doloribus porro amet velit. Repudiandae sunt provident perferendis necessitatibus debitis a fugiat.</t>
+  </si>
+  <si>
+    <t>Quas architecto assumenda rem et distinctio. Minus quaerat itaque ratione labore soluta earum. Omnis architecto ipsam vel assumenda.</t>
+  </si>
+  <si>
+    <t>désignation de modele action Eos accusamus modi recusandae ipsum. Dolorem quae dolores enim minima pariatur pariatur veniam. Ratione et velit. Aliquid molestiae nemo. Atque qui dolor enim aut optio ipsam aliquid.</t>
+  </si>
+  <si>
+    <t>Velit eos ut. Quia ut neque ut quia ut. Sunt sed numquam debitis sapiente molestias.</t>
+  </si>
+  <si>
+    <t>désignation action Delectus et commodi repudiandae vitae laboriosam voluptas. Animi soluta aut. Commodi voluptates sapiente. Qui inventore officiis laborum dolores.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-09T10:06:13.946337700</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-10T15:54:54.190552900</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-10T16:42:15.283776700</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-10T16:52:00.317965600</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-10T18:41:54.263719500</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T17:31:36.681309</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T17:48:33.576068500</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T17:59:53.243152</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T18:08:09.141836400</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T18:16:57.304050800</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T22:09:53.544771400</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-11T23:38:48.589039900</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-12T00:06:00.170276300</t>
+  </si>
+  <si>
+    <t>désignation action Tempore tenetur aut mollitia accusantium quia officia debitis. Accusamus aut voluptatem est optio. Enim iure impedit est ullam explicabo. Doloremque assumenda vitae omnis. Quia iusto consequuntur ipsa nihil saepe dolores.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-12T00:16:23.284824500</t>
+  </si>
+  <si>
+    <t>désignation action Quibusdam aliquid architecto exercitationem velit cumque eligendi itaque. Perferendis commodi accusantium optio labore occaecati molestias. Id quos accusantium neque. Occaecati eveniet amet eos cum. Ut soluta sed nisi placeat rerum.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-12T00:32:50.959102700</t>
+  </si>
+  <si>
+    <t>désignation action Exercitationem consequuntur laborum consequuntur inventore ut ipsa voluptas. Hic ex dolorem tenetur assumenda et. Ut qui ullam fuga aut. Doloribus rerum qui praesentium quasi odio doloremque architecto.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-12T00:50:33.475144100</t>
+  </si>
+  <si>
+    <t>désignation action Saepe dolor deleniti. Fuga totam magnam. Suscipit et deleniti id nihil. Possimus sit reiciendis cum nisi aut. Quod nesciunt odit id debitis laborum minima.</t>
   </si>
 </sst>
 </file>
@@ -3582,7 +3657,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId80"/>
+    <hyperlink ref="A2" r:id="rId105"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -11696,8 +11771,8 @@
       <c r="A2" t="s">
         <v>593</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>594</v>
+      <c r="B2" t="s">
+        <v>813</v>
       </c>
       <c r="C2" t="s">
         <v>596</v>
@@ -11728,7 +11803,7 @@
         <v>536</v>
       </c>
       <c r="M2" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>572</v>
@@ -11746,7 +11821,7 @@
         <v>575</v>
       </c>
       <c r="S2" t="s">
-        <v>783</v>
+        <v>814</v>
       </c>
       <c r="T2" t="s">
         <v>616</v>
@@ -11767,7 +11842,7 @@
         <v>91</v>
       </c>
       <c r="Z2" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="AA2" s="79" t="s">
         <v>582</v>
@@ -11809,7 +11884,7 @@
         <v>536</v>
       </c>
       <c r="M3" t="s">
-        <v>785</v>
+        <v>793</v>
       </c>
       <c r="N3" s="31" t="s">
         <v>583</v>
@@ -11827,7 +11902,7 @@
         <v>587</v>
       </c>
       <c r="S3" t="s">
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="T3" t="s">
         <v>616</v>
@@ -11848,7 +11923,7 @@
         <v>91</v>
       </c>
       <c r="Z3" t="s">
-        <v>784</v>
+        <v>792</v>
       </c>
       <c r="AA3" s="79" t="s">
         <v>580</v>

</xml_diff>

<commit_message>
add  test automation  for  module  action
</commit_message>
<xml_diff>
--- a/resources/testData/TestData.xlsx
+++ b/resources/testData/TestData.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="833">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2528,6 +2528,60 @@
   </si>
   <si>
     <t>désignation action Saepe dolor deleniti. Fuga totam magnam. Suscipit et deleniti id nihil. Possimus sit reiciendis cum nisi aut. Quod nesciunt odit id debitis laborum minima.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-13T00:25:24.094979600</t>
+  </si>
+  <si>
+    <t>désignation action Sed ea exercitationem vero rerum et. Veritatis laboriosam molestiae velit velit quis ad. Culpa occaecati similique.</t>
+  </si>
+  <si>
+    <t>désignation action Vitae voluptates enim error facere. Est autem eum. In perspiciatis veniam reprehenderit rerum sed sapiente eveniet.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-14T15:00:30.616825500</t>
+  </si>
+  <si>
+    <t>désignation action Et aspernatur qui sit aut minima veritatis. Sint est placeat laborum. Praesentium sit odit voluptate commodi quia tempore.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-14T19:15:45.496905700</t>
+  </si>
+  <si>
+    <t>désignation action Omnis ducimus nesciunt alias dicta corporis sed quisquam. Velit repellat dolorem excepturi earum voluptatem eaque non. Numquam et rerum quaerat repudiandae fugit. Perferendis similique aut est voluptas tempore assumenda.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-25T17:22:21.912096900</t>
+  </si>
+  <si>
+    <t>désignation action Rerum est officiis nobis quia sit laboriosam quo. Iusto quia impedit. Fuga et commodi voluptate. Dolorem aperiam exercitationem.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-26T00:19:44.967055900</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-26T00:57:35.632518</t>
+  </si>
+  <si>
+    <t>désignation action Ut quaerat est est. Quam molestiae ipsa soluta ea molestiae beatae minus. Amet laboriosam voluptatem beatae perspiciatis ab et.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-27T12:42:29.765941500</t>
+  </si>
+  <si>
+    <t>désignation action Id consectetur et. Optio molestias cum non. Animi quo non sed a saepe voluptatem. Consequatur possimus omnis odio ipsam.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-27T12:53:24.079695400</t>
+  </si>
+  <si>
+    <t>désignation action Libero alias ex reprehenderit accusamus aut amet dolorem. Omnis rerum sint repellat quo. Reprehenderit placeat eum ut. Laudantium quia temporibus qui at quia fugiat. Quaerat harum sed provident aut eius.</t>
+  </si>
+  <si>
+    <t>Type Action Auto2023-06-27T15:11:50.942705900</t>
+  </si>
+  <si>
+    <t>désignation action Et neque recusandae distinctio voluptatem molestiae ipsa. Officiis numquam libero. Est nostrum tempore voluptatem. Aliquam ut voluptas aut aut non quia dolores.</t>
   </si>
 </sst>
 </file>
@@ -3657,7 +3711,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId105"/>
+    <hyperlink ref="A2" r:id="rId123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -11772,7 +11826,7 @@
         <v>593</v>
       </c>
       <c r="B2" t="s">
-        <v>813</v>
+        <v>831</v>
       </c>
       <c r="C2" t="s">
         <v>596</v>
@@ -11821,7 +11875,7 @@
         <v>575</v>
       </c>
       <c r="S2" t="s">
-        <v>814</v>
+        <v>832</v>
       </c>
       <c r="T2" t="s">
         <v>616</v>

</xml_diff>

<commit_message>
demande action  et action simplifier
</commit_message>
<xml_diff>
--- a/resources/testData/TestData.xlsx
+++ b/resources/testData/TestData.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="870">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2687,6 +2687,12 @@
   </si>
   <si>
     <t>désignation action Dolores ut nesciunt. Ea consequuntur aliquam tempora consectetur non. Ipsam aut cum dolorum. Aut est est.</t>
+  </si>
+  <si>
+    <t>désignation action Quas quaerat nesciunt. Et aperiam voluptatem commodi. Itaque commodi quia deserunt qui dolor. Repellendus animi id voluptatem.</t>
+  </si>
+  <si>
+    <t>désignation action Repellendus minus eum non. Maxime delectus doloribus pariatur aut rem totam iste. Facilis earum sunt necessitatibus pariatur ad voluptates non. Ea minima expedita commodi. Consequuntur qui ratione voluptatibus inventore.</t>
   </si>
 </sst>
 </file>
@@ -3816,7 +3822,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId158"/>
+    <hyperlink ref="A2" r:id="rId160"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -11980,7 +11986,7 @@
         <v>575</v>
       </c>
       <c r="S2" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="T2" t="s">
         <v>616</v>

</xml_diff>